<commit_message>
Altera ordem processo SEI
</commit_message>
<xml_diff>
--- a/data-raw/DE_PARA.xlsx
+++ b/data-raw/DE_PARA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fjunior/Local/github/transparencia-mg/dt-contratacoes-coronavirus/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA19E0F-B74E-A146-88AD-EA5392D598E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920E30D4-4D7C-C844-AA32-94A03A0B19C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="15540" xr2:uid="{4EA3D1F0-8A75-3549-B7CC-51A81452A4EA}"/>
+    <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{4EA3D1F0-8A75-3549-B7CC-51A81452A4EA}"/>
   </bookViews>
   <sheets>
     <sheet name="mapeamento" sheetId="2" r:id="rId1"/>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8291C637-62C6-C945-A2A2-29C51C8E558C}">
   <dimension ref="B1:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22:C42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1348,7 +1348,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B32" sqref="B32:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1374,14 +1374,14 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
       </c>
       <c r="D2" t="str">
-        <f>B2</f>
-        <v>PROCESSO_SEI</v>
+        <f t="shared" ref="D2:D33" si="0">B2</f>
+        <v>NUMERO_PROCESSO_COMPRA</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1389,14 +1389,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D33" si="0">B3</f>
-        <v>URL_PROCESSO_SEI</v>
+        <f t="shared" si="0"/>
+        <v>URL_PORTAL_TRANSPARENCIA</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1404,14 +1404,14 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>NUMERO_PROCESSO_COMPRA</v>
+        <v>DATA_CADASTRAMENTO_PROCESSO</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1419,14 +1419,14 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>73</v>
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
-        <v>URL_PORTAL_TRANSPARENCIA</v>
+        <v>OBJETO_PROCESSO</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1434,14 +1434,14 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
+        <v>74</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
-        <v>DATA_CADASTRAMENTO_PROCESSO</v>
+        <v>URL_DOCUMENTOS_PROCESSO</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1449,14 +1449,14 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>OBJETO_PROCESSO</v>
+        <v>CODIGO_ORGAO_DEMANDANTE</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1464,14 +1464,14 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>74</v>
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
-        <v>URL_DOCUMENTOS_PROCESSO</v>
+        <v>ORGAO_DEMANDANTE</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1479,14 +1479,14 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>CODIGO_ORGAO_DEMANDANTE</v>
+        <v>SITUACAO_PROCESSO</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1494,14 +1494,14 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
-        <v>ORGAO_DEMANDANTE</v>
+        <v>PROCEDIMENTO_CONTRATACAO</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1509,14 +1509,14 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
-        <v>SITUACAO_PROCESSO</v>
+        <v>NUMERO_CONTRATO</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1524,14 +1524,14 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>PROCEDIMENTO_CONTRATACAO</v>
+        <v>URL_INTEGRA_CONTRATO</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1539,14 +1539,14 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>NUMERO_CONTRATO</v>
+        <v>CODIGO_ORGAO_CONTRATO</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1554,14 +1554,14 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
-        <v>URL_INTEGRA_CONTRATO</v>
+        <v>ORGAO_CONTRATO</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1569,14 +1569,14 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>CODIGO_ORGAO_CONTRATO</v>
+        <v>DATA_PUBLICACAO</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1584,14 +1584,14 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>ORGAO_CONTRATO</v>
+        <v>INICIO_VIGENCIA</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1599,14 +1599,14 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>DATA_PUBLICACAO</v>
+        <v>FIM_VIGENCIA</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1614,14 +1614,14 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>INICIO_VIGENCIA</v>
+        <v>FIM_VIGENCIA_ATUALIZADA</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1629,14 +1629,14 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>FIM_VIGENCIA</v>
+        <v>CNPJ_CPF_CONTRATADO</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1644,14 +1644,14 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>FIM_VIGENCIA_ATUALIZADA</v>
+        <v>CONTRATADO</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1659,14 +1659,14 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>CNPJ_CPF_CONTRATADO</v>
+        <f>B21</f>
+        <v>PROCESSO_SEI</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1674,14 +1674,14 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>16</v>
+        <v>72</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>CONTRATADO</v>
+        <f>B22</f>
+        <v>URL_PROCESSO_SEI</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>